<commit_message>
update pada bagian spi
</commit_message>
<xml_diff>
--- a/BackEnd_RMA/uploads/SPI.xlsx
+++ b/BackEnd_RMA/uploads/SPI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Madya Kuliah\Semester 7\PT DI\BackEnd_RMA\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496638A5-9CF9-4455-B3F7-C3C8E79725FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F237FB2-BDEB-4710-A760-73AF5F21EEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3624" yWindow="4332" windowWidth="17280" windowHeight="12600" xr2:uid="{8C6427D0-B0C2-4D4B-AB94-AF9B666D475E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8C6427D0-B0C2-4D4B-AB94-AF9B666D475E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Data &amp; Document Needed</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>qwer</t>
+  </si>
+  <si>
+    <t>20/09/2024'</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D01ED12-D89E-4B71-803E-21DF90698FDF}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,7 +518,9 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" t="s">
         <v>17</v>
       </c>
@@ -539,7 +544,9 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
@@ -563,7 +570,9 @@
       <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F4" t="s">
         <v>17</v>
       </c>
@@ -587,7 +596,9 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
@@ -611,7 +622,9 @@
       <c r="C6">
         <v>2</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
@@ -635,7 +648,9 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" t="s">
         <v>17</v>
       </c>

</xml_diff>